<commit_message>
ollama is working !!!
</commit_message>
<xml_diff>
--- a/input/Recipe_Search_Questions.xlsx
+++ b/input/Recipe_Search_Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\Fgv\7p_projetos\Search_Engine\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F128401C-78E2-45F8-A9E3-46B5FDD86998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E532D97D-67D7-47AB-B01C-11CEF4B7CC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="52">
   <si>
     <t>Tipo</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>I'm vegan. How can I make a bolognese?</t>
+  </si>
+  <si>
+    <t>I have 9min maximum to make a lunch, can you help me?</t>
+  </si>
+  <si>
+    <t>Esfiha de carne vegana</t>
   </si>
 </sst>
 </file>
@@ -532,15 +538,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -562,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -573,7 +579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -584,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -595,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -606,7 +612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -617,7 +623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -628,7 +634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -639,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -650,7 +656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -661,7 +667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -672,7 +678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -683,7 +689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -694,7 +700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -705,7 +711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -716,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -727,7 +733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -738,7 +744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -749,7 +755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -760,7 +766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -771,7 +777,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -782,7 +788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -793,7 +799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -804,7 +810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -815,7 +821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -826,7 +832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -837,7 +843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -848,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -859,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -870,7 +876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -881,7 +887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -892,7 +898,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -903,7 +909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -914,7 +920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -925,7 +931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -936,7 +942,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -947,7 +953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -958,7 +964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -969,7 +975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -980,7 +986,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -991,7 +997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1000,6 +1006,28 @@
       </c>
       <c r="C42" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>